<commit_message>
subido todo los archivos
</commit_message>
<xml_diff>
--- a/DEV/Microservicios-Product-app/Categories-cotroller/US3_CP_DEV_1.xlsx
+++ b/DEV/Microservicios-Product-app/Categories-cotroller/US3_CP_DEV_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\OneDrive\Escritorio\DOCUMENTOS\DEV\Microservicios-Product-app\Categories-cotroller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C08478-E633-47DC-A16E-6C68CA842213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0542BD21-6452-4118-9B38-626C1EA9E397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F7989457-68F4-4A2A-B67F-64262A68E569}"/>
   </bookViews>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEFDFD0-32E2-4D6C-ACEB-3E52EFAD76E5}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>